<commit_message>
End to End Test suite
</commit_message>
<xml_diff>
--- a/templates/AutomationOrg/FinancialData_AutomationOrg.xlsx
+++ b/templates/AutomationOrg/FinancialData_AutomationOrg.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Namrata\git\rsqasampleproj\templates\AutomationOrg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ABD0DE7-D7DA-488A-99ED-52E63D79C2A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46DEF308-7B23-4451-B600-CBBFF2CCD73A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{B6C21A89-21B4-4624-A955-66D166717697}"/>
   </bookViews>
   <sheets>
     <sheet name="Invoice" sheetId="15" r:id="rId1"/>
     <sheet name="BankDetail" sheetId="16" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="17" r:id="rId3"/>
-    <sheet name="JournalEntriesD" sheetId="18" r:id="rId4"/>
-    <sheet name="JournalEntries" sheetId="19" r:id="rId5"/>
+    <sheet name="ObjectName" sheetId="20" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="17" r:id="rId4"/>
+    <sheet name="JournalEntriesD" sheetId="18" r:id="rId5"/>
+    <sheet name="JournalEntries" sheetId="19" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
   <si>
     <t>Vendor</t>
   </si>
@@ -104,6 +105,30 @@
   </si>
   <si>
     <t>aBT5f000000wmqI</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>GLAccount</t>
+  </si>
+  <si>
+    <t>Fiscalyear</t>
+  </si>
+  <si>
+    <t>BankName</t>
+  </si>
+  <si>
+    <t>Mountain Manufacturing (100)</t>
+  </si>
+  <si>
+    <t>6655 (BC)</t>
+  </si>
+  <si>
+    <t>SB-24808 (1103)</t>
+  </si>
+  <si>
+    <t>Bank of Dad</t>
   </si>
 </sst>
 </file>
@@ -551,10 +576,66 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2EE9618-729B-4B79-83BE-CA1B6FCEE5EB}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2">
+        <v>2022</v>
+      </c>
+      <c r="E2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BEC8942-3B81-4719-B47B-7D8E287A86DD}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -583,7 +664,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF28B4E6-0495-4E52-B25E-8C3A3E173311}">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -637,7 +718,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F7E54B2-B7B4-44D4-8D7C-1B0233FCC129}">
   <dimension ref="A1:B3"/>
   <sheetViews>

</xml_diff>

<commit_message>
Inventory Requisition to Post Payment API
</commit_message>
<xml_diff>
--- a/templates/AutomationOrg/FinancialData_AutomationOrg.xlsx
+++ b/templates/AutomationOrg/FinancialData_AutomationOrg.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Namrata\git\rsqasampleproj\templates\AutomationOrg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46DEF308-7B23-4451-B600-CBBFF2CCD73A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10EE275E-BD4C-438E-8AAE-35E47EDF44C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{B6C21A89-21B4-4624-A955-66D166717697}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{B6C21A89-21B4-4624-A955-66D166717697}"/>
   </bookViews>
   <sheets>
     <sheet name="Invoice" sheetId="15" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
   <si>
     <t>Vendor</t>
   </si>
@@ -129,6 +129,18 @@
   </si>
   <si>
     <t>Bank of Dad</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>Division</t>
+  </si>
+  <si>
+    <t>100 Home Project</t>
+  </si>
+  <si>
+    <t>Colorado (100)</t>
   </si>
 </sst>
 </file>
@@ -577,10 +589,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2EE9618-729B-4B79-83BE-CA1B6FCEE5EB}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="F1" sqref="F1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,9 +602,10 @@
     <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -608,8 +621,14 @@
       <c r="E1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -624,6 +643,12 @@
       </c>
       <c r="E2" t="s">
         <v>29</v>
+      </c>
+      <c r="F2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PO Clean up updated the existing TC
</commit_message>
<xml_diff>
--- a/templates/AutomationOrg/FinancialData_AutomationOrg.xlsx
+++ b/templates/AutomationOrg/FinancialData_AutomationOrg.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Namrata\git\rsqasampleproj\templates\AutomationOrg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10EE275E-BD4C-438E-8AAE-35E47EDF44C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98BA2303-7FCA-4FD1-8F2C-4A27C5389CE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{B6C21A89-21B4-4624-A955-66D166717697}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="5" xr2:uid="{B6C21A89-21B4-4624-A955-66D166717697}"/>
   </bookViews>
   <sheets>
     <sheet name="Invoice" sheetId="15" r:id="rId1"/>
@@ -18,9 +18,11 @@
     <sheet name="ObjectName" sheetId="20" r:id="rId3"/>
     <sheet name="Sheet1" sheetId="17" r:id="rId4"/>
     <sheet name="JournalEntriesD" sheetId="18" r:id="rId5"/>
-    <sheet name="JournalEntries" sheetId="19" r:id="rId6"/>
+    <sheet name="GLAccount" sheetId="21" r:id="rId6"/>
+    <sheet name="JournalEntries" sheetId="19" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <t>Vendor</t>
   </si>
@@ -141,6 +143,12 @@
   </si>
   <si>
     <t>Colorado (100)</t>
+  </si>
+  <si>
+    <t>Account Name</t>
+  </si>
+  <si>
+    <t>2000 (Accounts Payable)</t>
   </si>
 </sst>
 </file>
@@ -591,8 +599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2EE9618-729B-4B79-83BE-CA1B6FCEE5EB}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:G1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -694,7 +702,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -744,6 +752,35 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59AB72CF-BF1E-4FC8-81CA-91352CC5A1BE}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F7E54B2-B7B4-44D4-8D7C-1B0233FCC129}">
   <dimension ref="A1:B3"/>
   <sheetViews>

</xml_diff>

<commit_message>
Account Payable TC update
</commit_message>
<xml_diff>
--- a/templates/AutomationOrg/FinancialData_AutomationOrg.xlsx
+++ b/templates/AutomationOrg/FinancialData_AutomationOrg.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Namrata\git\rsqasampleproj\templates\AutomationOrg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98BA2303-7FCA-4FD1-8F2C-4A27C5389CE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEAEF3EA-F562-4C74-BB60-3538EF3F678F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="5" xr2:uid="{B6C21A89-21B4-4624-A955-66D166717697}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="3" activeTab="8" xr2:uid="{B6C21A89-21B4-4624-A955-66D166717697}"/>
   </bookViews>
   <sheets>
     <sheet name="Invoice" sheetId="15" r:id="rId1"/>
@@ -20,9 +20,10 @@
     <sheet name="JournalEntriesD" sheetId="18" r:id="rId5"/>
     <sheet name="GLAccount" sheetId="21" r:id="rId6"/>
     <sheet name="JournalEntries" sheetId="19" r:id="rId7"/>
+    <sheet name="APATO" sheetId="22" r:id="rId8"/>
+    <sheet name="APATO_ForeignCurr" sheetId="23" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="48">
   <si>
     <t>Vendor</t>
   </si>
@@ -149,6 +150,42 @@
   </si>
   <si>
     <t>2000 (Accounts Payable)</t>
+  </si>
+  <si>
+    <t>PayType</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>PostPayTrans</t>
+  </si>
+  <si>
+    <t>LoadPosted</t>
+  </si>
+  <si>
+    <t>Check</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>Vendor Credit</t>
+  </si>
+  <si>
+    <t>Vendor Debit</t>
+  </si>
+  <si>
+    <t>Closed</t>
+  </si>
+  <si>
+    <t>BC Vendor INR (1097)</t>
   </si>
 </sst>
 </file>
@@ -755,7 +792,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59AB72CF-BF1E-4FC8-81CA-91352CC5A1BE}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -820,4 +857,1017 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31FAA796-8BBC-430B-911F-CF5C933DE15D}">
+  <dimension ref="A1:K14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2">
+        <v>650</v>
+      </c>
+      <c r="G2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2">
+        <v>2022</v>
+      </c>
+      <c r="I2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3">
+        <v>300</v>
+      </c>
+      <c r="G3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3">
+        <v>2022</v>
+      </c>
+      <c r="I3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4">
+        <v>300</v>
+      </c>
+      <c r="G4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4">
+        <v>2022</v>
+      </c>
+      <c r="I4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4" t="b">
+        <v>1</v>
+      </c>
+      <c r="K4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5">
+        <v>300</v>
+      </c>
+      <c r="G5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5">
+        <v>2022</v>
+      </c>
+      <c r="I5" t="s">
+        <v>44</v>
+      </c>
+      <c r="J5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6">
+        <v>300</v>
+      </c>
+      <c r="G6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H6">
+        <v>2022</v>
+      </c>
+      <c r="I6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J6" t="b">
+        <v>1</v>
+      </c>
+      <c r="K6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7">
+        <v>300</v>
+      </c>
+      <c r="G7" t="s">
+        <v>43</v>
+      </c>
+      <c r="H7">
+        <v>2022</v>
+      </c>
+      <c r="I7" t="s">
+        <v>45</v>
+      </c>
+      <c r="J7" t="b">
+        <v>0</v>
+      </c>
+      <c r="K7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8">
+        <v>300</v>
+      </c>
+      <c r="G8" t="s">
+        <v>43</v>
+      </c>
+      <c r="H8">
+        <v>2022</v>
+      </c>
+      <c r="I8" t="s">
+        <v>45</v>
+      </c>
+      <c r="J8" t="b">
+        <v>1</v>
+      </c>
+      <c r="K8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9">
+        <v>300</v>
+      </c>
+      <c r="G9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H9">
+        <v>2022</v>
+      </c>
+      <c r="I9" t="s">
+        <v>3</v>
+      </c>
+      <c r="J9" t="b">
+        <v>0</v>
+      </c>
+      <c r="K9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10">
+        <v>300</v>
+      </c>
+      <c r="G10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H10">
+        <v>2022</v>
+      </c>
+      <c r="I10" t="s">
+        <v>3</v>
+      </c>
+      <c r="J10" t="b">
+        <v>1</v>
+      </c>
+      <c r="K10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11">
+        <v>300</v>
+      </c>
+      <c r="G11" t="s">
+        <v>46</v>
+      </c>
+      <c r="H11">
+        <v>2022</v>
+      </c>
+      <c r="I11" t="s">
+        <v>44</v>
+      </c>
+      <c r="J11" t="b">
+        <v>0</v>
+      </c>
+      <c r="K11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12">
+        <v>300</v>
+      </c>
+      <c r="G12" t="s">
+        <v>46</v>
+      </c>
+      <c r="H12">
+        <v>2022</v>
+      </c>
+      <c r="I12" t="s">
+        <v>44</v>
+      </c>
+      <c r="J12" t="b">
+        <v>1</v>
+      </c>
+      <c r="K12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13">
+        <v>300</v>
+      </c>
+      <c r="G13" t="s">
+        <v>46</v>
+      </c>
+      <c r="H13">
+        <v>2022</v>
+      </c>
+      <c r="I13" t="s">
+        <v>45</v>
+      </c>
+      <c r="J13" t="b">
+        <v>0</v>
+      </c>
+      <c r="K13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14">
+        <v>300</v>
+      </c>
+      <c r="G14" t="s">
+        <v>46</v>
+      </c>
+      <c r="H14">
+        <v>2022</v>
+      </c>
+      <c r="I14" t="s">
+        <v>45</v>
+      </c>
+      <c r="J14" t="b">
+        <v>1</v>
+      </c>
+      <c r="K14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{882C5C1C-008A-463E-90A6-A2765E214EF6}">
+  <dimension ref="A1:K14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:R1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="11" max="11" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2">
+        <v>650</v>
+      </c>
+      <c r="G2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2">
+        <v>2022</v>
+      </c>
+      <c r="I2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3">
+        <v>300</v>
+      </c>
+      <c r="G3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3">
+        <v>2022</v>
+      </c>
+      <c r="I3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4">
+        <v>300</v>
+      </c>
+      <c r="G4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4">
+        <v>2022</v>
+      </c>
+      <c r="I4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4" t="b">
+        <v>1</v>
+      </c>
+      <c r="K4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5">
+        <v>300</v>
+      </c>
+      <c r="G5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5">
+        <v>2022</v>
+      </c>
+      <c r="I5" t="s">
+        <v>44</v>
+      </c>
+      <c r="J5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6">
+        <v>300</v>
+      </c>
+      <c r="G6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H6">
+        <v>2022</v>
+      </c>
+      <c r="I6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J6" t="b">
+        <v>1</v>
+      </c>
+      <c r="K6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7">
+        <v>300</v>
+      </c>
+      <c r="G7" t="s">
+        <v>43</v>
+      </c>
+      <c r="H7">
+        <v>2022</v>
+      </c>
+      <c r="I7" t="s">
+        <v>45</v>
+      </c>
+      <c r="J7" t="b">
+        <v>0</v>
+      </c>
+      <c r="K7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8">
+        <v>300</v>
+      </c>
+      <c r="G8" t="s">
+        <v>43</v>
+      </c>
+      <c r="H8">
+        <v>2022</v>
+      </c>
+      <c r="I8" t="s">
+        <v>45</v>
+      </c>
+      <c r="J8" t="b">
+        <v>1</v>
+      </c>
+      <c r="K8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9">
+        <v>300</v>
+      </c>
+      <c r="G9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H9">
+        <v>2022</v>
+      </c>
+      <c r="I9" t="s">
+        <v>3</v>
+      </c>
+      <c r="J9" t="b">
+        <v>0</v>
+      </c>
+      <c r="K9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10">
+        <v>300</v>
+      </c>
+      <c r="G10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H10">
+        <v>2022</v>
+      </c>
+      <c r="I10" t="s">
+        <v>3</v>
+      </c>
+      <c r="J10" t="b">
+        <v>1</v>
+      </c>
+      <c r="K10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11">
+        <v>300</v>
+      </c>
+      <c r="G11" t="s">
+        <v>46</v>
+      </c>
+      <c r="H11">
+        <v>2022</v>
+      </c>
+      <c r="I11" t="s">
+        <v>44</v>
+      </c>
+      <c r="J11" t="b">
+        <v>0</v>
+      </c>
+      <c r="K11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12">
+        <v>300</v>
+      </c>
+      <c r="G12" t="s">
+        <v>46</v>
+      </c>
+      <c r="H12">
+        <v>2022</v>
+      </c>
+      <c r="I12" t="s">
+        <v>44</v>
+      </c>
+      <c r="J12" t="b">
+        <v>1</v>
+      </c>
+      <c r="K12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13">
+        <v>300</v>
+      </c>
+      <c r="G13" t="s">
+        <v>46</v>
+      </c>
+      <c r="H13">
+        <v>2022</v>
+      </c>
+      <c r="I13" t="s">
+        <v>45</v>
+      </c>
+      <c r="J13" t="b">
+        <v>0</v>
+      </c>
+      <c r="K13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14">
+        <v>300</v>
+      </c>
+      <c r="G14" t="s">
+        <v>46</v>
+      </c>
+      <c r="H14">
+        <v>2022</v>
+      </c>
+      <c r="I14" t="s">
+        <v>45</v>
+      </c>
+      <c r="J14" t="b">
+        <v>1</v>
+      </c>
+      <c r="K14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
AP API Test Cases
</commit_message>
<xml_diff>
--- a/templates/AutomationOrg/FinancialData_AutomationOrg.xlsx
+++ b/templates/AutomationOrg/FinancialData_AutomationOrg.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Namrata\git\rsqasampleproj\templates\AutomationOrg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEAEF3EA-F562-4C74-BB60-3538EF3F678F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1AE6796-4099-49CA-826A-76131E6AECFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="3" activeTab="8" xr2:uid="{B6C21A89-21B4-4624-A955-66D166717697}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="8" activeTab="12" xr2:uid="{B6C21A89-21B4-4624-A955-66D166717697}"/>
   </bookViews>
   <sheets>
     <sheet name="Invoice" sheetId="15" r:id="rId1"/>
@@ -22,6 +22,10 @@
     <sheet name="JournalEntries" sheetId="19" r:id="rId7"/>
     <sheet name="APATO" sheetId="22" r:id="rId8"/>
     <sheet name="APATO_ForeignCurr" sheetId="23" r:id="rId9"/>
+    <sheet name="PAYTO" sheetId="24" r:id="rId10"/>
+    <sheet name="PAYTO_ForeignCurr" sheetId="25" r:id="rId11"/>
+    <sheet name="PAYTO_VCApplication" sheetId="26" r:id="rId12"/>
+    <sheet name="JEATO" sheetId="27" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="55">
   <si>
     <t>Vendor</t>
   </si>
@@ -186,6 +190,27 @@
   </si>
   <si>
     <t>BC Vendor INR (1097)</t>
+  </si>
+  <si>
+    <t>Bank Card</t>
+  </si>
+  <si>
+    <t>Cash</t>
+  </si>
+  <si>
+    <t>Payment</t>
+  </si>
+  <si>
+    <t>Vendor Credit Application</t>
+  </si>
+  <si>
+    <t>PAYTOTransType</t>
+  </si>
+  <si>
+    <t>SB BOI</t>
+  </si>
+  <si>
+    <t>CompanyNumber</t>
   </si>
 </sst>
 </file>
@@ -223,10 +248,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -578,7 +603,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2">
@@ -600,6 +625,598 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{350462E3-3517-4B38-B33B-9FE14DAEE19F}">
+  <dimension ref="A1:L5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" t="s">
+        <v>52</v>
+      </c>
+      <c r="L1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2">
+        <v>460</v>
+      </c>
+      <c r="G2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3">
+        <v>230</v>
+      </c>
+      <c r="G3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" t="b">
+        <v>1</v>
+      </c>
+      <c r="J3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4">
+        <v>340</v>
+      </c>
+      <c r="G4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" t="b">
+        <v>1</v>
+      </c>
+      <c r="J4" t="b">
+        <v>0</v>
+      </c>
+      <c r="K4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5">
+        <v>340</v>
+      </c>
+      <c r="G5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K5" t="s">
+        <v>50</v>
+      </c>
+      <c r="L5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B9CDD26-B41D-4543-BC56-5F3C36AEF6D3}">
+  <dimension ref="A1:L5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:L5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" t="s">
+        <v>52</v>
+      </c>
+      <c r="L1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2">
+        <v>20</v>
+      </c>
+      <c r="G2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3">
+        <v>30</v>
+      </c>
+      <c r="G3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" t="b">
+        <v>1</v>
+      </c>
+      <c r="J3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4">
+        <v>45</v>
+      </c>
+      <c r="G4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" t="b">
+        <v>1</v>
+      </c>
+      <c r="J4" t="b">
+        <v>0</v>
+      </c>
+      <c r="K4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5">
+        <v>200</v>
+      </c>
+      <c r="G5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K5" t="s">
+        <v>50</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE49A1E5-47B9-4DC7-A4D7-3817370716E5}">
+  <dimension ref="A1:K3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2">
+        <v>550</v>
+      </c>
+      <c r="G2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3">
+        <v>550</v>
+      </c>
+      <c r="G3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I3" t="b">
+        <v>1</v>
+      </c>
+      <c r="J3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D73858B1-E161-4780-831A-195B32325E97}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>100</v>
+      </c>
+      <c r="B2">
+        <v>200</v>
+      </c>
+      <c r="C2">
+        <v>200</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -637,7 +1254,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -772,7 +1389,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>16</v>
       </c>
       <c r="B3">
@@ -839,7 +1456,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="b">
+      <c r="A2" s="1" t="b">
         <v>0</v>
       </c>
       <c r="B2" t="s">
@@ -847,7 +1464,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="b">
+      <c r="A3" s="1" t="b">
         <v>1</v>
       </c>
       <c r="B3" t="s">
@@ -864,10 +1481,13 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="J12" sqref="J12:L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="9" max="9" width="21.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1368,8 +1988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{882C5C1C-008A-463E-90A6-A2765E214EF6}">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:R1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>